<commit_message>
Update of SOP for MI artifacts in measurement spreadsheet
</commit_message>
<xml_diff>
--- a/StateOfPractice/DomainMeasurements/MedImaging-Ao/MedicalImaging_Combined_MeasurementTemplate_EmpiricalMeasures.xlsx
+++ b/StateOfPractice/DomainMeasurements/MedImaging-Ao/MedicalImaging_Combined_MeasurementTemplate_EmpiricalMeasures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smiths/Repos/AIMSS/StateOfPractice/DomainMeasurements/MedImaging-Ao/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E5B5E8-81A5-A045-86D4-F6AC3A0453DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3EFBD8B-0DC0-394E-B851-D992B0087F32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28260" yWindow="3500" windowWidth="21020" windowHeight="21500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1000" yWindow="880" windowWidth="42800" windowHeight="21500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2289" uniqueCount="663">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2290" uniqueCount="663">
   <si>
     <t>Metrics &amp; Description</t>
   </si>
@@ -3347,12 +3347,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="AF117" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="A72" sqref="A72"/>
-      <selection pane="topRight" activeCell="B72" sqref="B72"/>
-      <selection pane="bottomLeft" activeCell="A74" sqref="A74"/>
-      <selection pane="bottomRight" activeCell="AG138" sqref="AG138"/>
+    <sheetView tabSelected="1" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
+      <pane xSplit="1" ySplit="4" topLeftCell="Z112" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="AE137" sqref="AE137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -13530,7 +13529,7 @@
         <v>627</v>
       </c>
       <c r="AF129">
-        <f>COUNTA(B129:AE129)</f>
+        <f t="shared" ref="AF129:AF137" si="3">COUNTA(B129:AE129)</f>
         <v>8</v>
       </c>
       <c r="AG129" t="s">
@@ -13575,7 +13574,7 @@
         <v>627</v>
       </c>
       <c r="AF130">
-        <f>COUNTA(B130:AE130)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="AG130" t="s">
@@ -13623,7 +13622,7 @@
         <v>627</v>
       </c>
       <c r="AF131">
-        <f>COUNTA(B131:AE131)</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="AG131" t="s">
@@ -13635,7 +13634,7 @@
         <v>622</v>
       </c>
       <c r="AF132">
-        <f>COUNTA(B132:AE132)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -13665,7 +13664,7 @@
         <v>627</v>
       </c>
       <c r="AF133">
-        <f>COUNTA(B133:AE133)</f>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="AG133" t="s">
@@ -13680,7 +13679,7 @@
         <v>627</v>
       </c>
       <c r="AF134">
-        <f>COUNTA(B134:AE134)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AG134" t="s">
@@ -13701,7 +13700,7 @@
         <v>627</v>
       </c>
       <c r="AF135">
-        <f>COUNTA(B135:AE135)</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="AG135" t="s">
@@ -13721,6 +13720,9 @@
       <c r="N136" t="s">
         <v>627</v>
       </c>
+      <c r="Q136" t="s">
+        <v>627</v>
+      </c>
       <c r="R136" t="s">
         <v>627</v>
       </c>
@@ -13740,8 +13742,8 @@
         <v>627</v>
       </c>
       <c r="AF136">
-        <f>COUNTA(B136:AE136)</f>
-        <v>9</v>
+        <f t="shared" si="3"/>
+        <v>10</v>
       </c>
       <c r="AG136" t="s">
         <v>661</v>
@@ -13767,7 +13769,7 @@
         <v>627</v>
       </c>
       <c r="AF137">
-        <f>COUNTA(B137:AE137)</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="AG137" t="s">

</xml_diff>